<commit_message>
Arreglo en la emisión de varios vehiculos. Scripts de emisión de póliza complementaria y blanket
</commit_message>
<xml_diff>
--- a/Sura/Emisión Motor - Varios vehiculos - General.xlsx
+++ b/Sura/Emisión Motor - Varios vehiculos - General.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443FBF66-3C14-4249-B40B-D80766942C07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5153D281-F66D-4ACD-B3FF-779657BCA230}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D7F8E601-CE60-45FC-A996-B80C264DA3F5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
   <si>
     <t>Ambiente</t>
   </si>
@@ -87,18 +87,9 @@
     <t>Menos de 5 vehículos</t>
   </si>
   <si>
-    <t>3 meses</t>
-  </si>
-  <si>
     <t>Cupón</t>
   </si>
   <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>3 Cuotas - ARS</t>
-  </si>
-  <si>
     <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
   </si>
   <si>
@@ -108,7 +99,31 @@
     <t>gw</t>
   </si>
   <si>
-    <t>14/01/2022</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Anual</t>
+  </si>
+  <si>
+    <t>CodigoAgente</t>
+  </si>
+  <si>
+    <t>NUM_GRUPO</t>
+  </si>
+  <si>
+    <t>Baioni Alejandro Luis</t>
+  </si>
+  <si>
+    <t>idEjecucion</t>
+  </si>
+  <si>
+    <t>01/03/2020</t>
+  </si>
+  <si>
+    <t>08/03/2020</t>
+  </si>
+  <si>
+    <t>21/03/2020</t>
   </si>
 </sst>
 </file>
@@ -159,11 +174,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -479,115 +495,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D847928-91FB-4604-8528-B7709C02B602}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <v>1067</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="3">
+        <v>8892807402</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="T2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>6188</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="3">
+        <v>8892807402</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3">
-        <v>7557632631</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>1067</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="3">
+        <v>8892807402</v>
+      </c>
+      <c r="I4" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>27</v>
+      <c r="F5">
+        <v>4994</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3">
+        <v>8892807402</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="Q3" s="1"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>234</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="3">
+        <v>8892807402</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>4994</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="3">
+        <v>8892807402</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8">
+        <v>234</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3">
+        <v>8892807402</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B8E024B4-2C90-4F11-9BE5-D103BFD66265}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2BB163F3-0500-4A89-9706-C2E61EABDAA5}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{0D21DA79-1FD7-4BBE-981A-5091ED136A36}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{5089F56B-2241-47FD-BD9D-5B7B9589C0AD}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{E54DD23F-D394-4359-BDE0-279562EFA05F}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{39A6B662-0BC2-406C-8291-B8567497A687}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{2E521C6E-578D-41EA-9A39-290C4571FC90}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{85CAAC0C-27E5-4928-95DC-2CE6813E3492}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ultimos cambios para pull
</commit_message>
<xml_diff>
--- a/Sura/Emisión Motor - Varios vehiculos - General.xlsx
+++ b/Sura/Emisión Motor - Varios vehiculos - General.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5153D281-F66D-4ACD-B3FF-779657BCA230}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F61FFF0-934B-443A-B0CA-7CCB807725B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D7F8E601-CE60-45FC-A996-B80C264DA3F5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Ambiente</t>
   </si>
@@ -111,19 +111,19 @@
     <t>NUM_GRUPO</t>
   </si>
   <si>
-    <t>Baioni Alejandro Luis</t>
-  </si>
-  <si>
     <t>idEjecucion</t>
   </si>
   <si>
-    <t>01/03/2020</t>
-  </si>
-  <si>
-    <t>08/03/2020</t>
-  </si>
-  <si>
-    <t>21/03/2020</t>
+    <t>Mattioli Luis Federico</t>
+  </si>
+  <si>
+    <t>SNP</t>
+  </si>
+  <si>
+    <t>2590036310073126210014</t>
+  </si>
+  <si>
+    <t>27/03/2023</t>
   </si>
 </sst>
 </file>
@@ -495,20 +495,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D847928-91FB-4604-8528-B7709C02B602}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -585,13 +586,13 @@
         <v>23</v>
       </c>
       <c r="F2">
-        <v>1067</v>
+        <v>2302</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H2" s="3">
-        <v>8892807402</v>
+        <v>4672846545</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -608,8 +609,9 @@
       <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="4" t="s">
-        <v>30</v>
+      <c r="Q2" s="1"/>
+      <c r="T2" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -629,13 +631,13 @@
         <v>23</v>
       </c>
       <c r="F3">
-        <v>6188</v>
+        <v>2302</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3" s="3">
-        <v>8892807402</v>
+        <v>4672846545</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -652,241 +654,46 @@
       <c r="M3" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="R3" t="s">
         <v>30</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4">
-        <v>1067</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="3">
-        <v>8892807402</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="T4" s="4"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5">
-        <v>4994</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="3">
-        <v>8892807402</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" t="s">
-        <v>24</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="T5" s="4"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6">
-        <v>234</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="3">
-        <v>8892807402</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" t="s">
-        <v>24</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="T6" s="4"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7">
-        <v>4994</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="3">
-        <v>8892807402</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" t="s">
-        <v>24</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8">
-        <v>234</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="3">
-        <v>8892807402</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" t="s">
-        <v>24</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="T7" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{2BB163F3-0500-4A89-9706-C2E61EABDAA5}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{0D21DA79-1FD7-4BBE-981A-5091ED136A36}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{5089F56B-2241-47FD-BD9D-5B7B9589C0AD}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{E54DD23F-D394-4359-BDE0-279562EFA05F}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{39A6B662-0BC2-406C-8291-B8567497A687}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{2E521C6E-578D-41EA-9A39-290C4571FC90}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{85CAAC0C-27E5-4928-95DC-2CE6813E3492}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{13F9388F-B4FD-4A1F-882A-F07F413FE408}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>